<commit_message>
WBS word2vec 부분 공란변경
</commit_message>
<xml_diff>
--- a/doc/[라떼는말이야]프로젝트_WBS.xlsx
+++ b/doc/[라떼는말이야]프로젝트_WBS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\issuewhatshow\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01.dev\git\issuewhatshow\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="176">
   <si>
     <t>공정</t>
   </si>
@@ -731,10 +731,6 @@
   </si>
   <si>
     <t>통합 분석기 소스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>word2vec 분석 코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -939,6 +935,18 @@
   </si>
   <si>
     <t>The Freedom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1331,6 +1339,54 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1354,54 +1410,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1683,13 +1691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD153"/>
+  <dimension ref="A1:XFD156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="4" topLeftCell="R35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1711,46 +1719,46 @@
       <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="39"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="31"/>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="37">
+      <c r="J1" s="56"/>
+      <c r="K1" s="53">
         <v>43771</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
       <c r="AB1" s="32"/>
-      <c r="AC1" s="56" t="s">
+      <c r="AC1" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD1" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="AD1" s="56" t="s">
+      <c r="AE1" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="AE1" s="56" t="s">
+      <c r="AF1" s="42" t="s">
         <v>165</v>
-      </c>
-      <c r="AF1" s="56" t="s">
-        <v>166</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>48</v>
@@ -1789,37 +1797,37 @@
       <c r="Z2" s="30"/>
       <c r="AA2" s="30"/>
       <c r="AB2" s="24"/>
-      <c r="AC2" s="59"/>
-      <c r="AD2" s="57"/>
-      <c r="AE2" s="58"/>
-      <c r="AF2" s="60"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="46"/>
       <c r="AH2" s="7"/>
       <c r="AI2" s="16"/>
       <c r="AJ2" s="8"/>
     </row>
     <row r="3" spans="1:53" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="54" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -1959,14 +1967,14 @@
       </c>
     </row>
     <row r="4" spans="1:53" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="6">
         <v>43731</v>
       </c>
@@ -2104,10 +2112,10 @@
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="13">
@@ -2179,19 +2187,19 @@
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="60"/>
+      <c r="B6" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="13">
-        <f t="shared" ref="C6:C43" si="0">IF(($K$1-F6+1)/E6&gt;=1,1,IF(($K$1-F6+1)/E6&lt;0,0, ($K$1-F6+1)/E6))</f>
+        <f t="shared" ref="C6:C46" si="0">IF(($K$1-F6+1)/E6&gt;=1,1,IF(($K$1-F6+1)/E6&lt;0,0, ($K$1-F6+1)/E6))</f>
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" ref="E6:E49" si="1">G6+1-F6</f>
+        <f t="shared" ref="E6:E46" si="1">G6+1-F6</f>
         <v>1</v>
       </c>
       <c r="F6" s="4">
@@ -2252,8 +2260,8 @@
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="60"/>
+      <c r="B7" s="38" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="13">
@@ -2325,8 +2333,8 @@
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="37" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="13">
@@ -2398,8 +2406,8 @@
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45" t="s">
+      <c r="A9" s="60"/>
+      <c r="B9" s="37" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="13">
@@ -2407,7 +2415,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="1"/>
@@ -2471,8 +2479,8 @@
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="46" t="s">
+      <c r="A10" s="60"/>
+      <c r="B10" s="38" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="13">
@@ -2480,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" s="10">
         <f t="shared" si="1"/>
@@ -2544,9 +2552,9 @@
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45" t="s">
-        <v>135</v>
+      <c r="A11" s="60"/>
+      <c r="B11" s="37" t="s">
+        <v>134</v>
       </c>
       <c r="C11" s="13">
         <f t="shared" si="0"/>
@@ -2617,8 +2625,8 @@
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="46" t="s">
+      <c r="A12" s="60"/>
+      <c r="B12" s="38" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="13">
@@ -2626,7 +2634,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12" s="10">
         <f t="shared" si="1"/>
@@ -2690,8 +2698,8 @@
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A13" s="44"/>
-      <c r="B13" s="46" t="s">
+      <c r="A13" s="60"/>
+      <c r="B13" s="38" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="13">
@@ -2699,7 +2707,7 @@
         <v>0.75</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="1"/>
@@ -2763,8 +2771,8 @@
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="37" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="13">
@@ -2772,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14" s="10">
         <f t="shared" si="1"/>
@@ -2836,8 +2844,8 @@
       </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="60"/>
+      <c r="B15" s="37" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="13">
@@ -2845,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="10">
         <f t="shared" si="1"/>
@@ -2912,7 +2920,7 @@
       <c r="A16" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="39" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="13"/>
@@ -3045,7 +3053,7 @@
     <row r="18" spans="1:53 16384:16384" x14ac:dyDescent="0.3">
       <c r="A18" s="51"/>
       <c r="B18" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" s="13">
         <f t="shared" si="0"/>
@@ -3190,8 +3198,8 @@
     </row>
     <row r="20" spans="1:53 16384:16384" x14ac:dyDescent="0.3">
       <c r="A20" s="51"/>
-      <c r="B20" s="48" t="s">
-        <v>125</v>
+      <c r="B20" s="40" t="s">
+        <v>124</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="5"/>
@@ -3250,7 +3258,7 @@
     </row>
     <row r="21" spans="1:53 16384:16384" x14ac:dyDescent="0.3">
       <c r="A21" s="51"/>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="41" t="s">
         <v>115</v>
       </c>
       <c r="C21" s="13"/>
@@ -3375,7 +3383,7 @@
         <f>IF(($K$1-F23+1)/E23&gt;=1,1,IF(($K$1-F23+1)/E23&lt;0,0, ($K$1-F23+1)/E23))</f>
         <v>1</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="47" t="s">
         <v>107</v>
       </c>
       <c r="E23" s="10">
@@ -3448,7 +3456,7 @@
         <f>IF(($K$1-F24+1)/E24&gt;=1,1,IF(($K$1-F24+1)/E24&lt;0,0, ($K$1-F24+1)/E24))</f>
         <v>1</v>
       </c>
-      <c r="D24" s="54"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3519,7 +3527,7 @@
         <f>IF(($K$1-F25+1)/E25&gt;=1,1,IF(($K$1-F25+1)/E25&lt;0,0, ($K$1-F25+1)/E25))</f>
         <v>1</v>
       </c>
-      <c r="D25" s="54"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3590,7 +3598,7 @@
         <f>IF(($K$1-F26+1)/E26&gt;=1,1,IF(($K$1-F26+1)/E26&lt;0,0, ($K$1-F26+1)/E26))</f>
         <v>1</v>
       </c>
-      <c r="D26" s="55"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3720,7 +3728,7 @@
         <f>IF(($K$1-F28+1)/E28&gt;=1,1,IF(($K$1-F28+1)/E28&lt;0,0, ($K$1-F28+1)/E28))</f>
         <v>1</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="D28" s="47" t="s">
         <v>108</v>
       </c>
       <c r="E28" s="10">
@@ -3793,7 +3801,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3805,7 +3813,7 @@
         <v>43739</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
@@ -3864,7 +3872,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D30" s="54"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3876,7 +3884,7 @@
         <v>43739</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
@@ -3935,7 +3943,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D31" s="55"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3947,7 +3955,7 @@
         <v>43739</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
@@ -3999,7 +4007,7 @@
     </row>
     <row r="32" spans="1:53 16384:16384" x14ac:dyDescent="0.3">
       <c r="A32" s="51"/>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="41" t="s">
         <v>116</v>
       </c>
       <c r="C32" s="13"/>
@@ -4065,7 +4073,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="D33" s="47" t="s">
         <v>120</v>
       </c>
       <c r="E33" s="10">
@@ -4138,7 +4146,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D34" s="54"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4209,7 +4217,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D35" s="54"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4280,7 +4288,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D36" s="55"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4344,8 +4352,8 @@
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A37" s="51"/>
-      <c r="B37" s="49" t="s">
-        <v>139</v>
+      <c r="B37" s="41" t="s">
+        <v>138</v>
       </c>
       <c r="C37" s="13">
         <f t="shared" si="0"/>
@@ -4417,8 +4425,8 @@
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A38" s="51"/>
-      <c r="B38" s="49" t="s">
-        <v>140</v>
+      <c r="B38" s="41" t="s">
+        <v>139</v>
       </c>
       <c r="C38" s="13">
         <f t="shared" si="0"/>
@@ -4490,8 +4498,8 @@
     </row>
     <row r="39" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="51"/>
-      <c r="B39" s="49" t="s">
-        <v>141</v>
+      <c r="B39" s="41" t="s">
+        <v>140</v>
       </c>
       <c r="C39" s="13">
         <f t="shared" si="0"/>
@@ -4563,8 +4571,8 @@
     </row>
     <row r="40" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="51"/>
-      <c r="B40" s="49" t="s">
-        <v>142</v>
+      <c r="B40" s="41" t="s">
+        <v>141</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="5"/>
@@ -4625,26 +4633,12 @@
       <c r="B41" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="13">
-        <f t="shared" ref="C40:C41" si="2">IF(($K$1-F41+1)/E41&gt;=1,1,IF(($K$1-F41+1)/E41&lt;0,0, ($K$1-F41+1)/E41))</f>
-        <v>1</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="10">
-        <f t="shared" ref="E40:E41" si="3">G41+1-F41</f>
-        <v>10</v>
-      </c>
-      <c r="F41" s="4">
-        <v>43742</v>
-      </c>
-      <c r="G41" s="4">
-        <v>43751</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>112</v>
-      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="11"/>
       <c r="I41" s="21"/>
       <c r="J41" s="21"/>
       <c r="K41" s="21"/>
@@ -4656,16 +4650,16 @@
       <c r="Q41" s="21"/>
       <c r="R41" s="21"/>
       <c r="S41" s="21"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="8"/>
-      <c r="AB41" s="8"/>
-      <c r="AC41" s="8"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="21"/>
+      <c r="AC41" s="21"/>
       <c r="AD41" s="21"/>
       <c r="AE41" s="21"/>
       <c r="AF41" s="21"/>
@@ -4695,28 +4689,18 @@
     </row>
     <row r="42" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="51"/>
-      <c r="B42" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E42" s="10">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
+      <c r="B42" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="10"/>
       <c r="F42" s="4">
         <v>43742</v>
       </c>
-      <c r="G42" s="4">
-        <v>43751</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>114</v>
+      <c r="G42" s="4"/>
+      <c r="H42" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="I42" s="21"/>
       <c r="J42" s="21"/>
@@ -4729,16 +4713,16 @@
       <c r="Q42" s="21"/>
       <c r="R42" s="21"/>
       <c r="S42" s="21"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="8"/>
-      <c r="AA42" s="8"/>
-      <c r="AB42" s="8"/>
-      <c r="AC42" s="8"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="21"/>
+      <c r="Z42" s="21"/>
+      <c r="AA42" s="21"/>
+      <c r="AB42" s="21"/>
+      <c r="AC42" s="21"/>
       <c r="AD42" s="21"/>
       <c r="AE42" s="21"/>
       <c r="AF42" s="21"/>
@@ -4762,34 +4746,20 @@
       <c r="AX42" s="34"/>
       <c r="AY42" s="34"/>
       <c r="AZ42" s="34"/>
-      <c r="BA42" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="BA42" s="2"/>
     </row>
     <row r="43" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="51"/>
-      <c r="B43" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E43" s="10">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F43" s="4">
-        <v>43750</v>
-      </c>
-      <c r="G43" s="4">
-        <v>43751</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>92</v>
+      <c r="B43" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
@@ -4810,8 +4780,8 @@
       <c r="Y43" s="21"/>
       <c r="Z43" s="21"/>
       <c r="AA43" s="21"/>
-      <c r="AB43" s="8"/>
-      <c r="AC43" s="8"/>
+      <c r="AB43" s="21"/>
+      <c r="AC43" s="21"/>
       <c r="AD43" s="21"/>
       <c r="AE43" s="21"/>
       <c r="AF43" s="21"/>
@@ -4835,40 +4805,28 @@
       <c r="AX43" s="34"/>
       <c r="AY43" s="34"/>
       <c r="AZ43" s="34"/>
-      <c r="BA43" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="BA43" s="2"/>
     </row>
     <row r="44" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="51"/>
-      <c r="B44" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="13">
-        <f t="shared" ref="C44:C45" si="4">IF(($K$1-F44+1)/E44&gt;=1,1,IF(($K$1-F44+1)/E44&lt;0,0, ($K$1-F44+1)/E44))</f>
-        <v>1</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="10">
-        <f t="shared" ref="E44:E45" si="5">G44+1-F44</f>
-        <v>5</v>
-      </c>
-      <c r="F44" s="4">
-        <v>43752</v>
-      </c>
+      <c r="B44" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="4">
-        <v>43756</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
+        <v>43751</v>
+      </c>
+      <c r="H44" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
       <c r="N44" s="21"/>
       <c r="O44" s="21"/>
       <c r="P44" s="21"/>
@@ -4885,11 +4843,11 @@
       <c r="AA44" s="21"/>
       <c r="AB44" s="21"/>
       <c r="AC44" s="21"/>
-      <c r="AD44" s="8"/>
-      <c r="AE44" s="8"/>
-      <c r="AF44" s="8"/>
-      <c r="AG44" s="8"/>
-      <c r="AH44" s="8"/>
+      <c r="AD44" s="21"/>
+      <c r="AE44" s="21"/>
+      <c r="AF44" s="21"/>
+      <c r="AG44" s="21"/>
+      <c r="AH44" s="21"/>
       <c r="AI44" s="21"/>
       <c r="AJ44" s="21"/>
       <c r="AK44" s="21"/>
@@ -4908,42 +4866,54 @@
       <c r="AX44" s="34"/>
       <c r="AY44" s="34"/>
       <c r="AZ44" s="34"/>
-      <c r="BA44" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="BA44" s="2"/>
     </row>
     <row r="45" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="51"/>
-      <c r="B45" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
+      <c r="B45" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F45" s="4">
+        <v>43742</v>
+      </c>
+      <c r="G45" s="4">
+        <v>43751</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="21"/>
       <c r="Q45" s="21"/>
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
-      <c r="W45" s="21"/>
-      <c r="X45" s="21"/>
-      <c r="Y45" s="21"/>
-      <c r="Z45" s="21"/>
-      <c r="AA45" s="21"/>
-      <c r="AB45" s="21"/>
-      <c r="AC45" s="21"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="8"/>
+      <c r="Z45" s="8"/>
+      <c r="AA45" s="8"/>
+      <c r="AB45" s="8"/>
+      <c r="AC45" s="8"/>
       <c r="AD45" s="21"/>
       <c r="AE45" s="21"/>
       <c r="AF45" s="21"/>
@@ -4952,10 +4922,10 @@
       <c r="AI45" s="21"/>
       <c r="AJ45" s="21"/>
       <c r="AK45" s="21"/>
-      <c r="AL45" s="21"/>
-      <c r="AM45" s="21"/>
-      <c r="AN45" s="21"/>
-      <c r="AO45" s="21"/>
+      <c r="AL45" s="34"/>
+      <c r="AM45" s="34"/>
+      <c r="AN45" s="34"/>
+      <c r="AO45" s="34"/>
       <c r="AP45" s="34"/>
       <c r="AQ45" s="34"/>
       <c r="AR45" s="34"/>
@@ -4973,34 +4943,34 @@
     </row>
     <row r="46" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="51"/>
-      <c r="B46" s="19" t="s">
-        <v>137</v>
+      <c r="B46" s="20" t="s">
+        <v>125</v>
       </c>
       <c r="C46" s="13">
-        <f t="shared" ref="C46" si="6">IF(($K$1-F46+1)/E46&gt;=1,1,IF(($K$1-F46+1)/E46&lt;0,0, ($K$1-F46+1)/E46))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="E46" s="10">
-        <f t="shared" ref="E46:E49" si="7">G46+1-F46</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F46" s="4">
-        <v>43757</v>
+        <v>43750</v>
       </c>
       <c r="G46" s="4">
-        <v>43758</v>
-      </c>
-      <c r="H46" s="14" t="s">
+        <v>43751</v>
+      </c>
+      <c r="H46" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="21"/>
@@ -5015,15 +4985,15 @@
       <c r="Y46" s="21"/>
       <c r="Z46" s="21"/>
       <c r="AA46" s="21"/>
-      <c r="AB46" s="21"/>
-      <c r="AC46" s="21"/>
+      <c r="AB46" s="8"/>
+      <c r="AC46" s="8"/>
       <c r="AD46" s="21"/>
       <c r="AE46" s="21"/>
       <c r="AF46" s="21"/>
       <c r="AG46" s="21"/>
       <c r="AH46" s="21"/>
-      <c r="AI46" s="8"/>
-      <c r="AJ46" s="8"/>
+      <c r="AI46" s="21"/>
+      <c r="AJ46" s="21"/>
       <c r="AK46" s="21"/>
       <c r="AL46" s="34"/>
       <c r="AM46" s="34"/>
@@ -5046,28 +5016,28 @@
     </row>
     <row r="47" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="51"/>
-      <c r="B47" s="19" t="s">
-        <v>132</v>
+      <c r="B47" s="40" t="s">
+        <v>121</v>
       </c>
       <c r="C47" s="13">
-        <f>IF(($K$1-F47+1)/E47&gt;=1,1,IF(($K$1-F47+1)/E47&lt;0,0, ($K$1-F47+1)/E47))</f>
+        <f t="shared" ref="C47" si="2">IF(($K$1-F47+1)/E47&gt;=1,1,IF(($K$1-F47+1)/E47&lt;0,0, ($K$1-F47+1)/E47))</f>
         <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="E47" s="10">
-        <f t="shared" si="7"/>
-        <v>7</v>
+        <f t="shared" ref="E47" si="3">G47+1-F47</f>
+        <v>5</v>
       </c>
       <c r="F47" s="4">
-        <v>43757</v>
+        <v>43752</v>
       </c>
       <c r="G47" s="4">
-        <v>43763</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>102</v>
+        <v>43756</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
@@ -5090,18 +5060,18 @@
       <c r="AA47" s="21"/>
       <c r="AB47" s="21"/>
       <c r="AC47" s="21"/>
-      <c r="AD47" s="21"/>
-      <c r="AE47" s="21"/>
-      <c r="AF47" s="21"/>
-      <c r="AG47" s="21"/>
-      <c r="AH47" s="21"/>
-      <c r="AI47" s="8"/>
-      <c r="AJ47" s="8"/>
-      <c r="AK47" s="8"/>
-      <c r="AL47" s="8"/>
-      <c r="AM47" s="8"/>
-      <c r="AN47" s="8"/>
-      <c r="AO47" s="8"/>
+      <c r="AD47" s="8"/>
+      <c r="AE47" s="8"/>
+      <c r="AF47" s="8"/>
+      <c r="AG47" s="8"/>
+      <c r="AH47" s="8"/>
+      <c r="AI47" s="21"/>
+      <c r="AJ47" s="21"/>
+      <c r="AK47" s="21"/>
+      <c r="AL47" s="34"/>
+      <c r="AM47" s="34"/>
+      <c r="AN47" s="34"/>
+      <c r="AO47" s="34"/>
       <c r="AP47" s="34"/>
       <c r="AQ47" s="34"/>
       <c r="AR47" s="34"/>
@@ -5119,29 +5089,15 @@
     </row>
     <row r="48" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="51"/>
-      <c r="B48" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="13">
-        <f>IF(($K$1-F48+1)/E48&gt;=1,1,IF(($K$1-F48+1)/E48&lt;0,0, ($K$1-F48+1)/E48))</f>
-        <v>1</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E48" s="10">
-        <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="F48" s="4">
-        <v>43757</v>
-      </c>
-      <c r="G48" s="4">
-        <v>43763</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>112</v>
-      </c>
+      <c r="B48" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
@@ -5168,13 +5124,13 @@
       <c r="AF48" s="21"/>
       <c r="AG48" s="21"/>
       <c r="AH48" s="21"/>
-      <c r="AI48" s="8"/>
-      <c r="AJ48" s="8"/>
-      <c r="AK48" s="8"/>
-      <c r="AL48" s="8"/>
-      <c r="AM48" s="8"/>
-      <c r="AN48" s="8"/>
-      <c r="AO48" s="8"/>
+      <c r="AI48" s="21"/>
+      <c r="AJ48" s="21"/>
+      <c r="AK48" s="21"/>
+      <c r="AL48" s="21"/>
+      <c r="AM48" s="21"/>
+      <c r="AN48" s="21"/>
+      <c r="AO48" s="21"/>
       <c r="AP48" s="34"/>
       <c r="AQ48" s="34"/>
       <c r="AR48" s="34"/>
@@ -5193,27 +5149,27 @@
     <row r="49" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="51"/>
       <c r="B49" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C49" s="13">
-        <f>IF(($K$1-F49+1)/E49&gt;=1,1,IF(($K$1-F49+1)/E49&lt;0,0, ($K$1-F49+1)/E49))</f>
+        <f t="shared" ref="C49" si="4">IF(($K$1-F49+1)/E49&gt;=1,1,IF(($K$1-F49+1)/E49&lt;0,0, ($K$1-F49+1)/E49))</f>
         <v>1</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E49" s="10">
-        <f t="shared" si="7"/>
-        <v>7</v>
+        <f t="shared" ref="E49:E52" si="5">G49+1-F49</f>
+        <v>2</v>
       </c>
       <c r="F49" s="4">
         <v>43757</v>
       </c>
       <c r="G49" s="4">
-        <v>43763</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>133</v>
+        <v>43758</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -5243,11 +5199,11 @@
       <c r="AH49" s="21"/>
       <c r="AI49" s="8"/>
       <c r="AJ49" s="8"/>
-      <c r="AK49" s="8"/>
-      <c r="AL49" s="8"/>
-      <c r="AM49" s="8"/>
-      <c r="AN49" s="8"/>
-      <c r="AO49" s="8"/>
+      <c r="AK49" s="21"/>
+      <c r="AL49" s="34"/>
+      <c r="AM49" s="34"/>
+      <c r="AN49" s="34"/>
+      <c r="AO49" s="34"/>
       <c r="AP49" s="34"/>
       <c r="AQ49" s="34"/>
       <c r="AR49" s="34"/>
@@ -5266,27 +5222,27 @@
     <row r="50" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="51"/>
       <c r="B50" s="19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C50" s="13">
-        <f t="shared" ref="C50:C55" si="8">IF(($K$1-F50+1)/E50&gt;=1,1,IF(($K$1-F50+1)/E50&lt;0,0, ($K$1-F50+1)/E50))</f>
+        <f>IF(($K$1-F50+1)/E50&gt;=1,1,IF(($K$1-F50+1)/E50&lt;0,0, ($K$1-F50+1)/E50))</f>
         <v>1</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E50" s="10">
-        <f t="shared" ref="E50:E56" si="9">G50+1-F50</f>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="F50" s="4">
-        <v>43759</v>
+        <v>43757</v>
       </c>
       <c r="G50" s="4">
-        <v>43761</v>
-      </c>
-      <c r="H50" s="35" t="s">
-        <v>97</v>
+        <v>43763</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -5314,13 +5270,13 @@
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
       <c r="AH50" s="21"/>
-      <c r="AI50" s="21"/>
-      <c r="AJ50" s="21"/>
+      <c r="AI50" s="8"/>
+      <c r="AJ50" s="8"/>
       <c r="AK50" s="8"/>
       <c r="AL50" s="8"/>
       <c r="AM50" s="8"/>
-      <c r="AN50" s="34"/>
-      <c r="AO50" s="34"/>
+      <c r="AN50" s="8"/>
+      <c r="AO50" s="8"/>
       <c r="AP50" s="34"/>
       <c r="AQ50" s="34"/>
       <c r="AR50" s="34"/>
@@ -5339,27 +5295,27 @@
     <row r="51" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="51"/>
       <c r="B51" s="19" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C51" s="13">
-        <f t="shared" si="8"/>
+        <f>IF(($K$1-F51+1)/E51&gt;=1,1,IF(($K$1-F51+1)/E51&lt;0,0, ($K$1-F51+1)/E51))</f>
         <v>1</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E51" s="10">
-        <f t="shared" si="9"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="F51" s="4">
-        <v>43762</v>
+        <v>43757</v>
       </c>
       <c r="G51" s="4">
         <v>43763</v>
       </c>
-      <c r="H51" s="35" t="s">
-        <v>97</v>
+      <c r="H51" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -5387,11 +5343,11 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="21"/>
-      <c r="AJ51" s="21"/>
-      <c r="AK51" s="21"/>
-      <c r="AL51" s="34"/>
-      <c r="AM51" s="34"/>
+      <c r="AI51" s="8"/>
+      <c r="AJ51" s="8"/>
+      <c r="AK51" s="8"/>
+      <c r="AL51" s="8"/>
+      <c r="AM51" s="8"/>
       <c r="AN51" s="8"/>
       <c r="AO51" s="8"/>
       <c r="AP51" s="34"/>
@@ -5411,15 +5367,29 @@
     </row>
     <row r="52" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="51"/>
-      <c r="B52" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="35"/>
+      <c r="B52" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="13">
+        <f>IF(($K$1-F52+1)/E52&gt;=1,1,IF(($K$1-F52+1)/E52&lt;0,0, ($K$1-F52+1)/E52))</f>
+        <v>1</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="10">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="F52" s="4">
+        <v>43757</v>
+      </c>
+      <c r="G52" s="4">
+        <v>43763</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>132</v>
+      </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
@@ -5446,18 +5416,18 @@
       <c r="AF52" s="21"/>
       <c r="AG52" s="21"/>
       <c r="AH52" s="21"/>
-      <c r="AI52" s="21"/>
-      <c r="AJ52" s="21"/>
-      <c r="AK52" s="21"/>
-      <c r="AL52" s="34"/>
-      <c r="AM52" s="34"/>
-      <c r="AN52" s="34"/>
-      <c r="AO52" s="34"/>
-      <c r="AP52" s="21"/>
-      <c r="AQ52" s="21"/>
-      <c r="AR52" s="21"/>
-      <c r="AS52" s="21"/>
-      <c r="AT52" s="21"/>
+      <c r="AI52" s="8"/>
+      <c r="AJ52" s="8"/>
+      <c r="AK52" s="8"/>
+      <c r="AL52" s="8"/>
+      <c r="AM52" s="8"/>
+      <c r="AN52" s="8"/>
+      <c r="AO52" s="8"/>
+      <c r="AP52" s="34"/>
+      <c r="AQ52" s="34"/>
+      <c r="AR52" s="34"/>
+      <c r="AS52" s="34"/>
+      <c r="AT52" s="34"/>
       <c r="AU52" s="34"/>
       <c r="AV52" s="34"/>
       <c r="AW52" s="34"/>
@@ -5471,27 +5441,27 @@
     <row r="53" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="51"/>
       <c r="B53" s="19" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C53" s="13">
-        <f>IF(($K$1-F53+1)/E53&gt;=1,1,IF(($K$1-F53+1)/E53&lt;0,0, ($K$1-F53+1)/E53))</f>
+        <f t="shared" ref="C53:C54" si="6">IF(($K$1-F53+1)/E53&gt;=1,1,IF(($K$1-F53+1)/E53&lt;0,0, ($K$1-F53+1)/E53))</f>
         <v>1</v>
       </c>
-      <c r="D53" s="53" t="s">
-        <v>170</v>
+      <c r="D53" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E53" s="10">
-        <f t="shared" si="9"/>
-        <v>5</v>
+        <f t="shared" ref="E53:E59" si="7">G53+1-F53</f>
+        <v>3</v>
       </c>
       <c r="F53" s="4">
-        <v>43764</v>
+        <v>43759</v>
       </c>
       <c r="G53" s="4">
-        <v>43768</v>
+        <v>43761</v>
       </c>
       <c r="H53" s="35" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -5521,16 +5491,16 @@
       <c r="AH53" s="21"/>
       <c r="AI53" s="21"/>
       <c r="AJ53" s="21"/>
-      <c r="AK53" s="21"/>
-      <c r="AL53" s="34"/>
-      <c r="AM53" s="34"/>
+      <c r="AK53" s="8"/>
+      <c r="AL53" s="8"/>
+      <c r="AM53" s="8"/>
       <c r="AN53" s="34"/>
       <c r="AO53" s="34"/>
-      <c r="AP53" s="8"/>
-      <c r="AQ53" s="8"/>
-      <c r="AR53" s="8"/>
-      <c r="AS53" s="8"/>
-      <c r="AT53" s="8"/>
+      <c r="AP53" s="34"/>
+      <c r="AQ53" s="34"/>
+      <c r="AR53" s="34"/>
+      <c r="AS53" s="34"/>
+      <c r="AT53" s="34"/>
       <c r="AU53" s="34"/>
       <c r="AV53" s="34"/>
       <c r="AW53" s="34"/>
@@ -5544,25 +5514,27 @@
     <row r="54" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="51"/>
       <c r="B54" s="19" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="C54" s="13">
-        <f>IF(($K$1-F54+1)/E54&gt;=1,1,IF(($K$1-F54+1)/E54&lt;0,0, ($K$1-F54+1)/E54))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="D54" s="54"/>
+      <c r="D54" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="E54" s="10">
-        <f t="shared" si="9"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="F54" s="4">
-        <v>43764</v>
+        <v>43762</v>
       </c>
       <c r="G54" s="4">
-        <v>43768</v>
+        <v>43763</v>
       </c>
       <c r="H54" s="35" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
@@ -5595,13 +5567,13 @@
       <c r="AK54" s="21"/>
       <c r="AL54" s="34"/>
       <c r="AM54" s="34"/>
-      <c r="AN54" s="34"/>
-      <c r="AO54" s="34"/>
-      <c r="AP54" s="8"/>
-      <c r="AQ54" s="8"/>
-      <c r="AR54" s="8"/>
-      <c r="AS54" s="8"/>
-      <c r="AT54" s="8"/>
+      <c r="AN54" s="8"/>
+      <c r="AO54" s="8"/>
+      <c r="AP54" s="34"/>
+      <c r="AQ54" s="34"/>
+      <c r="AR54" s="34"/>
+      <c r="AS54" s="34"/>
+      <c r="AT54" s="34"/>
       <c r="AU54" s="34"/>
       <c r="AV54" s="34"/>
       <c r="AW54" s="34"/>
@@ -5614,27 +5586,15 @@
     </row>
     <row r="55" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="51"/>
-      <c r="B55" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C55" s="13">
-        <f>IF(($K$1-F55+1)/E55&gt;=1,1,IF(($K$1-F55+1)/E55&lt;0,0, ($K$1-F55+1)/E55))</f>
-        <v>1</v>
-      </c>
-      <c r="D55" s="54"/>
-      <c r="E55" s="10">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="F55" s="4">
-        <v>43764</v>
-      </c>
-      <c r="G55" s="4">
-        <v>43768</v>
-      </c>
-      <c r="H55" s="35" t="s">
-        <v>157</v>
-      </c>
+      <c r="B55" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="35"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
@@ -5668,11 +5628,11 @@
       <c r="AM55" s="34"/>
       <c r="AN55" s="34"/>
       <c r="AO55" s="34"/>
-      <c r="AP55" s="8"/>
-      <c r="AQ55" s="8"/>
-      <c r="AR55" s="8"/>
-      <c r="AS55" s="8"/>
-      <c r="AT55" s="8"/>
+      <c r="AP55" s="21"/>
+      <c r="AQ55" s="21"/>
+      <c r="AR55" s="21"/>
+      <c r="AS55" s="21"/>
+      <c r="AT55" s="21"/>
       <c r="AU55" s="34"/>
       <c r="AV55" s="34"/>
       <c r="AW55" s="34"/>
@@ -5686,15 +5646,17 @@
     <row r="56" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="51"/>
       <c r="B56" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C56" s="13">
-        <f>IF(($K$1-F56+1)/E56&gt;=1,1,IF(($K$1-F56+1)/E56&lt;0,0, ($K$1-F56+1)/E56))</f>
+        <f t="shared" ref="C56:C62" si="8">IF(($K$1-F56+1)/E56&gt;=1,1,IF(($K$1-F56+1)/E56&lt;0,0, ($K$1-F56+1)/E56))</f>
         <v>1</v>
       </c>
-      <c r="D56" s="55"/>
+      <c r="D56" s="47" t="s">
+        <v>169</v>
+      </c>
       <c r="E56" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="F56" s="4">
@@ -5704,7 +5666,7 @@
         <v>43768</v>
       </c>
       <c r="H56" s="35" t="s">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
@@ -5756,28 +5718,26 @@
     </row>
     <row r="57" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="51"/>
-      <c r="B57" s="48" t="s">
-        <v>154</v>
+      <c r="B57" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="C57" s="13">
-        <f>IF(($K$1-F57+1)/E57&gt;=1,1,IF(($K$1-F57+1)/E57&lt;0,0, ($K$1-F57+1)/E57))</f>
-        <v>0.75</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>162</v>
-      </c>
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D57" s="48"/>
       <c r="E57" s="10">
-        <f>G57+1-F57</f>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="F57" s="4">
-        <v>43769</v>
+        <v>43764</v>
       </c>
       <c r="G57" s="4">
-        <v>43772</v>
+        <v>43768</v>
       </c>
       <c r="H57" s="35" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
@@ -5812,15 +5772,15 @@
       <c r="AM57" s="34"/>
       <c r="AN57" s="34"/>
       <c r="AO57" s="34"/>
-      <c r="AP57" s="34"/>
-      <c r="AQ57" s="34"/>
-      <c r="AR57" s="34"/>
-      <c r="AS57" s="34"/>
-      <c r="AT57" s="34"/>
-      <c r="AU57" s="8"/>
-      <c r="AV57" s="8"/>
-      <c r="AW57" s="8"/>
-      <c r="AX57" s="8"/>
+      <c r="AP57" s="8"/>
+      <c r="AQ57" s="8"/>
+      <c r="AR57" s="8"/>
+      <c r="AS57" s="8"/>
+      <c r="AT57" s="8"/>
+      <c r="AU57" s="34"/>
+      <c r="AV57" s="34"/>
+      <c r="AW57" s="34"/>
+      <c r="AX57" s="34"/>
       <c r="AY57" s="34"/>
       <c r="AZ57" s="34"/>
       <c r="BA57" s="2" t="s">
@@ -5829,28 +5789,26 @@
     </row>
     <row r="58" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="51"/>
-      <c r="B58" s="48" t="s">
-        <v>155</v>
+      <c r="B58" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="C58" s="13">
-        <f>IF(($K$1-F58+1)/E58&gt;=1,1,IF(($K$1-F58+1)/E58&lt;0,0, ($K$1-F58+1)/E58))</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>152</v>
-      </c>
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="48"/>
       <c r="E58" s="10">
-        <f>G58+1-F58</f>
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="F58" s="4">
-        <v>43773</v>
+        <v>43764</v>
       </c>
       <c r="G58" s="4">
-        <v>43773</v>
+        <v>43768</v>
       </c>
       <c r="H58" s="35" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
@@ -5885,45 +5843,43 @@
       <c r="AM58" s="34"/>
       <c r="AN58" s="34"/>
       <c r="AO58" s="34"/>
-      <c r="AP58" s="34"/>
-      <c r="AQ58" s="34"/>
-      <c r="AR58" s="34"/>
-      <c r="AS58" s="34"/>
-      <c r="AT58" s="34"/>
+      <c r="AP58" s="8"/>
+      <c r="AQ58" s="8"/>
+      <c r="AR58" s="8"/>
+      <c r="AS58" s="8"/>
+      <c r="AT58" s="8"/>
       <c r="AU58" s="34"/>
       <c r="AV58" s="34"/>
       <c r="AW58" s="34"/>
       <c r="AX58" s="34"/>
-      <c r="AY58" s="8"/>
+      <c r="AY58" s="34"/>
       <c r="AZ58" s="34"/>
       <c r="BA58" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="52"/>
-      <c r="B59" s="48" t="s">
-        <v>151</v>
+      <c r="A59" s="51"/>
+      <c r="B59" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="C59" s="13">
-        <f>IF(($K$1-F59+1)/E59&gt;=1,1,IF(($K$1-F59+1)/E59&lt;0,0, ($K$1-F59+1)/E59))</f>
-        <v>0</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>173</v>
-      </c>
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="49"/>
       <c r="E59" s="10">
-        <f>G59+1-F59</f>
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="F59" s="4">
-        <v>43774</v>
+        <v>43764</v>
       </c>
       <c r="G59" s="4">
-        <v>43774</v>
+        <v>43768</v>
       </c>
       <c r="H59" s="35" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
@@ -5958,35 +5914,239 @@
       <c r="AM59" s="34"/>
       <c r="AN59" s="34"/>
       <c r="AO59" s="34"/>
-      <c r="AP59" s="34"/>
-      <c r="AQ59" s="34"/>
-      <c r="AR59" s="34"/>
-      <c r="AS59" s="34"/>
-      <c r="AT59" s="34"/>
+      <c r="AP59" s="8"/>
+      <c r="AQ59" s="8"/>
+      <c r="AR59" s="8"/>
+      <c r="AS59" s="8"/>
+      <c r="AT59" s="8"/>
       <c r="AU59" s="34"/>
       <c r="AV59" s="34"/>
       <c r="AW59" s="34"/>
       <c r="AX59" s="34"/>
       <c r="AY59" s="34"/>
-      <c r="AZ59" s="8"/>
+      <c r="AZ59" s="34"/>
       <c r="BA59" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="E60"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-    </row>
-    <row r="61" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="E61"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-    </row>
-    <row r="62" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="E62"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
+    <row r="60" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="51"/>
+      <c r="B60" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="13">
+        <f t="shared" si="8"/>
+        <v>0.75</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E60" s="10">
+        <f>G60+1-F60</f>
+        <v>4</v>
+      </c>
+      <c r="F60" s="4">
+        <v>43769</v>
+      </c>
+      <c r="G60" s="4">
+        <v>43772</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="21"/>
+      <c r="Q60" s="21"/>
+      <c r="R60" s="21"/>
+      <c r="S60" s="21"/>
+      <c r="T60" s="21"/>
+      <c r="U60" s="21"/>
+      <c r="V60" s="21"/>
+      <c r="W60" s="21"/>
+      <c r="X60" s="21"/>
+      <c r="Y60" s="21"/>
+      <c r="Z60" s="21"/>
+      <c r="AA60" s="21"/>
+      <c r="AB60" s="21"/>
+      <c r="AC60" s="21"/>
+      <c r="AD60" s="21"/>
+      <c r="AE60" s="21"/>
+      <c r="AF60" s="21"/>
+      <c r="AG60" s="21"/>
+      <c r="AH60" s="21"/>
+      <c r="AI60" s="21"/>
+      <c r="AJ60" s="21"/>
+      <c r="AK60" s="21"/>
+      <c r="AL60" s="34"/>
+      <c r="AM60" s="34"/>
+      <c r="AN60" s="34"/>
+      <c r="AO60" s="34"/>
+      <c r="AP60" s="34"/>
+      <c r="AQ60" s="34"/>
+      <c r="AR60" s="34"/>
+      <c r="AS60" s="34"/>
+      <c r="AT60" s="34"/>
+      <c r="AU60" s="8"/>
+      <c r="AV60" s="8"/>
+      <c r="AW60" s="8"/>
+      <c r="AX60" s="8"/>
+      <c r="AY60" s="34"/>
+      <c r="AZ60" s="34"/>
+      <c r="BA60" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="51"/>
+      <c r="B61" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="10">
+        <f>G61+1-F61</f>
+        <v>1</v>
+      </c>
+      <c r="F61" s="4">
+        <v>43773</v>
+      </c>
+      <c r="G61" s="4">
+        <v>43773</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="21"/>
+      <c r="Q61" s="21"/>
+      <c r="R61" s="21"/>
+      <c r="S61" s="21"/>
+      <c r="T61" s="21"/>
+      <c r="U61" s="21"/>
+      <c r="V61" s="21"/>
+      <c r="W61" s="21"/>
+      <c r="X61" s="21"/>
+      <c r="Y61" s="21"/>
+      <c r="Z61" s="21"/>
+      <c r="AA61" s="21"/>
+      <c r="AB61" s="21"/>
+      <c r="AC61" s="21"/>
+      <c r="AD61" s="21"/>
+      <c r="AE61" s="21"/>
+      <c r="AF61" s="21"/>
+      <c r="AG61" s="21"/>
+      <c r="AH61" s="21"/>
+      <c r="AI61" s="21"/>
+      <c r="AJ61" s="21"/>
+      <c r="AK61" s="21"/>
+      <c r="AL61" s="34"/>
+      <c r="AM61" s="34"/>
+      <c r="AN61" s="34"/>
+      <c r="AO61" s="34"/>
+      <c r="AP61" s="34"/>
+      <c r="AQ61" s="34"/>
+      <c r="AR61" s="34"/>
+      <c r="AS61" s="34"/>
+      <c r="AT61" s="34"/>
+      <c r="AU61" s="34"/>
+      <c r="AV61" s="34"/>
+      <c r="AW61" s="34"/>
+      <c r="AX61" s="34"/>
+      <c r="AY61" s="8"/>
+      <c r="AZ61" s="34"/>
+      <c r="BA61" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="52"/>
+      <c r="B62" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E62" s="10">
+        <f>G62+1-F62</f>
+        <v>1</v>
+      </c>
+      <c r="F62" s="4">
+        <v>43774</v>
+      </c>
+      <c r="G62" s="4">
+        <v>43774</v>
+      </c>
+      <c r="H62" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="21"/>
+      <c r="O62" s="21"/>
+      <c r="P62" s="21"/>
+      <c r="Q62" s="21"/>
+      <c r="R62" s="21"/>
+      <c r="S62" s="21"/>
+      <c r="T62" s="21"/>
+      <c r="U62" s="21"/>
+      <c r="V62" s="21"/>
+      <c r="W62" s="21"/>
+      <c r="X62" s="21"/>
+      <c r="Y62" s="21"/>
+      <c r="Z62" s="21"/>
+      <c r="AA62" s="21"/>
+      <c r="AB62" s="21"/>
+      <c r="AC62" s="21"/>
+      <c r="AD62" s="21"/>
+      <c r="AE62" s="21"/>
+      <c r="AF62" s="21"/>
+      <c r="AG62" s="21"/>
+      <c r="AH62" s="21"/>
+      <c r="AI62" s="21"/>
+      <c r="AJ62" s="21"/>
+      <c r="AK62" s="21"/>
+      <c r="AL62" s="34"/>
+      <c r="AM62" s="34"/>
+      <c r="AN62" s="34"/>
+      <c r="AO62" s="34"/>
+      <c r="AP62" s="34"/>
+      <c r="AQ62" s="34"/>
+      <c r="AR62" s="34"/>
+      <c r="AS62" s="34"/>
+      <c r="AT62" s="34"/>
+      <c r="AU62" s="34"/>
+      <c r="AV62" s="34"/>
+      <c r="AW62" s="34"/>
+      <c r="AX62" s="34"/>
+      <c r="AY62" s="34"/>
+      <c r="AZ62" s="8"/>
+      <c r="BA62" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="63" spans="1:53" x14ac:dyDescent="0.3">
       <c r="E63"/>
@@ -6009,14 +6169,17 @@
       <c r="G66" s="9"/>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E67"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E68"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E69"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
@@ -6356,13 +6519,23 @@
       <c r="F153" s="9"/>
       <c r="G153" s="9"/>
     </row>
+    <row r="154" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+    </row>
+    <row r="155" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+    </row>
+    <row r="156" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="A16:A59"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A15"/>
     <mergeCell ref="K1:AA1"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="F1:G1"/>
@@ -6372,9 +6545,11 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="A16:A62"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="D28:D31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>